<commit_message>
dataset changes and exp
</commit_message>
<xml_diff>
--- a/Library Management/dataset2/LibraryManagement_authentic_dataset.xlsx
+++ b/Library Management/dataset2/LibraryManagement_authentic_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/Library Management/dataset2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C315E-5C69-FC4D-80CB-4B167E0C3B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F145CB0F-E9C6-814B-A1CB-FAD596F59B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,9 +260,6 @@
     <t>module OM_name: 0, open Declaration one sig class1_name extends Class attrSet = c1_at1+c1_at2 id=c1_at1 no parent isAbstract = No } one sig c1_at1 extends c1_at1_type one sig c1_at2 extends c1_at2_type, one sig class2_name extends Class attrSet = c2_at1+c2_at2 id = c2_at1 no parent isAbstract = No } one sig c2_at1 extends c2_at1_type one sig c2_at2 extends c2_at2_type, one sig class3_name extends Class attrSet = c3_at1+c3_at2+c3_at3+c3_at4+c3_at5+c3_at6 id=c3_at1 no parent isAbstract = No } one sig c3_at1 extends c3_at1_type one sig c3_at2 extends c3_at2_type one sig c3_at3 extends c3_at3_type one sig c3_at4 extends c3_at4_type one sig c3_at5 extends c3_at5_type one sig c3_at6 extends c3_at6_type, one sig class4_name extends Class attrSet = c4_at1+c4_at2+c4_at3+c4_at4 id=c4_at3 no parent isAbstract = No } one sig c4_at1 extends c4_at1_type one sig c4_at2 extends c4_at2_type one sig c4_at3 extends c4_at3_type one sig c4_at4 extends c4_at4_type, one sig class5_name extends Class attrSet = c5_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c5_at1 extends c5_at1_type, one sig class6_name extends Class attrSet = c6_at1_0+c6_at2+c6_at3+c6_at4 id=c6_at2 no parent isAbstract = No } one sig c6_at1_0 extends c6_at1_type one sig c6_at2 extends c6_at2_type one sig c6_at3 extends c6_at3_type one sig c6_at4 extends c6_at4_type, one sig class7_name extends Class attrSet = c7_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c7_at1 extends c7_at1_type, one sig class8_name extends Class attrSet = c8_at1+c8_at2+c2_at2+c6_at3 id=c8_at1 no parent isAbstract = No } one sig c8_at1 extends c8_at1_type one sig c8_at1 extends c8_at1_type, one sig assoc1 extends Association src = class8_name dst = class2_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc2 extends Association src = class2_name dst = class4_name, src_multiplicity = src_mlpc2 dst_multiplicity = dst_mlpc, } one sig assoc3 extends Association src = class8_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc4 extends Association src = class8_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc5 extends Association src = class8_name dst = class6_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc6 extends Association src = class6_name dst = class1_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc7 extends Association src = class6_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc8 extends Association src = class1_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc9 extends Association src = class1_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc10 extends Association src = class2_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, }, MappingStrategyforclass1_name:map_str2MappingStrategyforclass3_name:map_str2MappingStrategyforclass5_name:map_str2MappingStrategyforclass6_name:map_str2MappingStrategyfoarclass7_name:map_str2AssociationStrategyforassoc1:assoc_str1AssociationStrategyforassoc9:assoc_str1AssociationStrategyforassoc10:assoc_str2AssociationStrategyforassoc3:assoc_str2AssociationStrategyforassoc4:assoc_str2AssociationStrategyforassoc5:assoc_str2AssociationStrategyforassoc6:assoc_str2AssociationStrategyforassoc7:assoc_str2AssociationStrategyforassoc8:assoc_str2​, USE OM_name_0 CREATE TABLE `class3_name` ( `c3_at6` c3_at6_type `c3_at5` c3_at5_type `c3_at4` c3_at4_type `c3_at3` c3_at3_type `c3_at2` c3_at2_type c3_at1` c3_at1_type NOT NULL PRIMARY KEY (`c3_at1`), ); CREATE TABLE `class1_name` ( `c1_at1` c1_at2_type(64) `c1_at1` c1_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class2_name` ( `c2_at2` c2_at2_type(64) `c8_at1` c8_at1_type c2_at1` c2_at1_type NOT NULL KEY `FK_class2_name_c8_at1_idx` (`c8_at1`) PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class7_name` ( `c7_at1` c7_at1_type(64) `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc10` ( c3_at1` c3_at1_type NOT NULL c2_at1` c2_at1_type NOT NULL KEY `FK_assoc10_c3_at1_idx` (`c3_at1`) KEY `FK_assoc10_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c3_at1`,`c2_at1`), ); CREATE TABLE `class8_name` ( `c8_at2` c8_at2_type(64) ``c8_at1` c8_at1_type NOT NULL PRIMARY KEY (`c8_at1`), ); CREATE TABLE `class5_name` ( `c5_at1` c5_at1_type, `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc7` ( `c2_at1` c2_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc7_c6_at2_idx` (`c6_at2`), KEY `FK_assoc7_c4_at3_idx` (`c4_at3`), PRIMARY KEY (`c6_at2`,`c4_at3`) ); CREATE TABLE `assoc5` ( ``c8_at1` c8_at1_type NOT NULL `c2_at1` c2_at1_type NOT NULL KEY `FK_assoc5_c8_at1_idx` (`c8_at1`), KEY `FK_assoc5_c6_at2_idx` (`c6_at2`) PRIMARY KEY (`c8_at1`,`c6_at2`), ); CREATE TABLE `assoc3` ( ``c8_at1` c8_at1_type NOT NULL c3_at1` c3_at1_type NOT NULL KEY `FK_assoc3_c8_at1_idx` (`c8_at1`) KEY `FK_assoc3_c3_at1_idx` (`c3_at1`) PRIMARY KEY (`c8_at1`,`c3_at1`) ); CREATE TABLE `assoc8` ( c3_at1` c3_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL KEY `FK_assoc8_c3_at1_idx` (`c3_at1`) KEY `FK_assoc8_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c3_at1`,`c1_at1`) ); CREATE TABLE `class4_name` ( `c4_at4` c4_at4_type(64) `c4_at2` c4_at2_type(64) `c4_at1` c4_at1_type(64) `c4_at3` c4_at3_type c1_at1` c1_at1_type KEY `FK_class4_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c4_at3`), ); CREATE TABLE `assoc4` ( ``c8_at1` c8_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc4_c8_at1_idx` (`c8_at1`) KEY `FK_assoc4_c4_at3_idx` (`c4_at3`) PRIMARY KEY (`c8_at1`,`c4_at3`) ); CREATE TABLE `assoc6` ( `c2_at1` c2_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL `c3_at1` c3_at1_type NOT NULL KEY `FK_assoc6_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c6_at2`,`c1_at1`), ); CREATE TABLE `class6_name` ( `c6_at4` c6_at4_type(64) `c6_at3` c6_at3_type(64) `c6_at1_0` c6_at1_type `c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c6_at2`), ); CREATE TABLE `assoc2` ( `c4_at3` c4_at3_type c2_at1` c2_at1_type NOT NULL KEY `FK_assoc2_c4_at3_idx` (`c4_at3`) KEY `FK_assoc2_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c4_at3`,`c2_at1`), ); ALTER TABLE `class2_name` ADD CONSTRAINT `FK_class2_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ALTER TABLE `assoc10` ADD CONSTRAINT `FK_assoc10_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ADD CONSTRAINT `FK_assoc10_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc7` ADD CONSTRAINT `FK_assoc7_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc7_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc5` ADD CONSTRAINT `FK_assoc5_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc5_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc3` ADD CONSTRAINT `FK_assoc3_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc3_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc8` ADD CONSTRAINT `FK_assoc8_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc8_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `class4_name` ADD CONSTRAINT `FK_class4_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc4` ADD CONSTRAINT `FK_assoc4_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc4_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc6` ADD CONSTRAINT `FK_assoc6_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc6_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc2` ADD CONSTRAINT `FK_assoc2_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc2_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE</t>
   </si>
   <si>
-    <t>module OM_name: 0, open Declaration one sig class1_name extends Class attrSet = c1_at1+c1_at2 id=c1_at1 no parent isAbstract = No } one sig c1_at1 extends c1_at1_type one sig c1_at2 extends c1_at2_type, one sig class2_name extends Class attrSet = c2_at1+c2_at2 id = c2_at1 no parent isAbstract = No } one sig c2_at1 extends c2_at1_type one sig c2_at2 extends c2_at2_type, one sig class3_name extends Class attrSet = c3_at1+c3_at2+c3_at3+c3_at4+c3_at5+c3_at6 id=c3_at1 no parent isAbstract = No } one sig c3_at1 extends c3_at1_type one sig c3_at2 extends c3_at2_type one sig c3_at3 extends c3_at3_type one sig c3_at4 extends c3_at4_type one sig c3_at5 extends c3_at5_type one sig c3_at6 extends c3_at6_type, one sig class4_name extends Class attrSet = c4_at1+c4_at2+c4_at3+c4_at4 id=c4_at3 no parent isAbstract = No } one sig c4_at1 extends c4_at1_type one sig c4_at2 extends c4_at2_type one sig c4_at3 extends c4_at3_type one sig c4_at4 extends c4_at4_type, one sig class5_name extends Class attrSet = c5_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c5_at1 extends c5_at1_type, one sig class6_name extends Class attrSet = c6_at1_0+c6_at2+c6_at3+c6_at4 id=c6_at2 no parent isAbstract = No } one sig c6_at1_0 extends c6_at1_type one sig c6_at2 extends c6_at2_type one sig c6_at3 extends c6_at3_type one sig c6_at4 extends c6_at4_type, one sig class7_name extends Class attrSet = c7_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c7_at1 extends c7_at1_type, one sig class8_name extends Class attrSet = c8_at1+c8_at2+c2_at2+c6_at3 id=c8_at1 no parent isAbstract = No } one sig c8_at1 extends c8_at1_type one sig c8_at1 extends c8_at1_type, one sig assoc1 extends Association src = class8_name dst = class2_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc2 extends Association src = class2_name dst = class4_name, src_multiplicity = src_mlpc2 dst_multiplicity = dst_mlpc, } one sig assoc3 extends Association src = class8_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc4 extends Association src = class8_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc5 extends Association src = class8_name dst = class6_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc6 extends Association src = class6_name dst = class1_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc7 extends Association src = class6_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc8 extends Association src = class1_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc9 extends Association src = class1_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc10 extends Association src = class2_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, }, MappingStrategyforclass1_name:map_str2MappingStrategyforclass3_name:map_str2MappingStrategyforclass5_name:map_str2MappingStrategyforclass6_name:map_str2MappingStrategyfoarclass7_name:map_str2AssociationStrategyforassoc1:assoc_str1AssociationStrategyforassoc9:assoc_str1AssociationStrategyforassoc10:assoc_str2AssociationStrategyforassoc3:assoc_str2AssociationStrategyforassoc4:assoc_str2AssociationStrategyforassoc5:assoc_str2AssociationStrategyforassoc6:assoc_str2AssociationStrategyforassoc7:assoc_str2AssociationStrategyforassoc8:assoc_str2​, USE OM_name_0 CREATE TABLE `class3_name` ( `c3_at6` c3_at6_type `c3_at5` c3_at5_type `c3_at4` c3_at4_type `c3_at3` c3_at3_type `c3_at2` c3_at2_type c3_at1` c3_at1_type NOT NULL PRIMARY KEY (`c3_at1`), ); CREATE TABLE `class1_name` ( `c1_at1` c1_at2_type(64) `c1_at1` c1_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class2_name` ( `c2_at2` c2_at2_type(64) `c8_at1` c8_at1_type c2_at1` c2_at1_type NOT NULL KEY `FK_class2_name_c8_at1_idx` (`c8_at1`) PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class7_name` ( `c7_at1` c7_at1_type(64) `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc10` ( c3_at1` c3_at1_type NOT NULL c2_at1` c2_at1_type NOT NULL KEY `FK_assoc10_c3_at1_idx` (`c3_at1`) KEY `FK_assoc10_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c3_at1`,`c2_at1`), ); CREATE TABLE `class8_name` ( `c8_at2` c8_at2_type(64) ``c8_at1` c8_at1_type NOT NULL PRIMARY KEY (`c8_at1`), ); CREATE TABLE `class5_name` ( `c5_at1` c5_at1_type, `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc7` ( `c2_at1` c2_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc7_c6_at2_idx` (`c6_at2`), KEY `FK_assoc7_c4_at3_idx` (`c4_at3`), PRIMARY KEY (`c6_at2`,`c4_at3`) ); CREATE TABLE `assoc5` ( ``c8_at1` c8_at1_type NOT NULL `c2_at1` c2_at1_type NOT NULL KEY `FK_assoc5_c8_at1_idx` (`c8_at1`), KEY `FK_assoc5_c6_at2_idx` (`c6_at2`) PRIMARY KEY (`c8_at1`,`c6_at2`), ); CREATE TABLE `assoc3` ( ``c8_at1` c8_at1_type NOT NULL c3_at1` c3_at1_type NOT NULL KEY `FK_assoc3_c8_at1_idx` (`c8_at1`) KEY `FK_assoc3_c3_at1_idx` (`c3_at1`) PRIMARY KEY (`c8_at1`,`c3_at1`) ); CREATE TABLE `assoc8` ( c3_at1` c3_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL KEY `FK_assoc8_c3_at1_idx` (`c3_at1`) KEY `FK_assoc8_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c3_at1`,`c1_at1`) ); CREATE TABLE `class4_name` ( `c4_at4` c4_at4_type(64) `c4_at2` c4_at2_type(64) `c4_at1` c4_at1_type(64) `c4_at3` c4_at3_type c1_at1` c1_at1_type KEY `FK_class4_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c4_at3`), ); CREATE TABLE `assoc4` ( ``c8_at1` c8_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc4_c8_at1_idx` (`c8_at1`) KEY `FK_assoc4_c4_at3_idx` (`c4_at3`) PRIMARY KEY (`c8_at1`,`c4_at3`) ); CREATE TABLE `assoc6` ( `c2_at1` c2_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL `c3_at1` c3_at1_type NOT NULL KEY `FK_assoc6_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c6_at2`,`c1_at1`), ); CREATE TABLE `class6_name` ( `c6_at4` c6_at4_type(64) `c6_at3` c6_at3_type(64) `c6_at1_0` c6_at1_type `c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c6_at2`), ); CREATE TABLE `assoc2` ( `c4_at3` c4_at3_type c2_at1` c2_at1_type NOT NULL KEY `FK_assoc2_c4_at3_idx` (`c4_at3`) KEY `FK_assoc2_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c4_at3`,`c2_at1`), ); ALTER TABLE `class2_name` ADD CONSTRAINT `FK_class2_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ALTER TABLE `assoc10` ADD CONSTRAINT `FK_assoc10_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ADD CONSTRAINT `FK_assoc10_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc7` ADD CONSTRAINT `FK_assoc7_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc7_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc5` ADD CONSTRAINT `FK_assoc5_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc5_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc3` ADD CONSTRAINT `FK_assoc3_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc3_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc8` ADD CONSTRAINT `FK_assoc8_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc8_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `class4_name` ADD CONSTRAINT `FK_class4_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc4` ADD CONSTRAINT `FK_assoc4_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc4_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc6` ADD CONSTRAINT `FK_assoc6_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc6_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc2` ADD CONSTRAINT `FK_assoc2_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc2_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE,NP</t>
-  </si>
-  <si>
     <t>module OM_name: 0, open Declaration one sig class1_name extends Class attrSet = c1_at1+c1_at2 id=c1_at1 no parent isAbstract = No } one sig c1_at1 extends c1_at1_type one sig c1_at2 extends c1_at2_type, one sig class2_name extends Class attrSet = c2_at1+c2_at2 id = c2_at1 no parent isAbstract = No } one sig c2_at1 extends c2_at1_type one sig c2_at2 extends c2_at2_type, one sig class3_name extends Class attrSet = c3_at1+c3_at2+c3_at3+c3_at4+c3_at5+c3_at6 id=c3_at1 no parent isAbstract = No } one sig c3_at1 extends c3_at1_type one sig c3_at2 extends c3_at2_type one sig c3_at3 extends c3_at3_type one sig c3_at4 extends c3_at4_type one sig c3_at5 extends c3_at5_type one sig c3_at6 extends c3_at6_type, one sig class4_name extends Class attrSet = c4_at1+c4_at2+c4_at3+c4_at4 id=c4_at3 no parent isAbstract = No } one sig c4_at1 extends c4_at1_type one sig c4_at2 extends c4_at2_type one sig c4_at3 extends c4_at3_type one sig c4_at4 extends c4_at4_type, one sig class5_name extends Class attrSet = c5_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c5_at1 extends c5_at1_type, one sig class6_name extends Class attrSet = c6_at1_0+c6_at2+c6_at3+c6_at4 id=c6_at2 no parent isAbstract = No } one sig c6_at1_0 extends c6_at1_type one sig c6_at2 extends c6_at2_type one sig c6_at3 extends c6_at3_type one sig c6_at4 extends c6_at4_type, one sig class7_name extends Class attrSet = c7_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c7_at1 extends c7_at1_type, one sig class8_name extends Class attrSet = c8_at1+c8_at2+c2_at2+c6_at3 id=c8_at1 no parent isAbstract = No } one sig c8_at1 extends c8_at1_type one sig c8_at1 extends c8_at1_type, one sig assoc1 extends Association src = class8_name dst = class2_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc2 extends Association src = class2_name dst = class4_name, src_multiplicity = src_mlpc2 dst_multiplicity = dst_mlpc, } one sig assoc3 extends Association src = class8_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc4 extends Association src = class8_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc5 extends Association src = class8_name dst = class6_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc6 extends Association src = class6_name dst = class1_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc7 extends Association src = class6_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc8 extends Association src = class1_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc9 extends Association src = class1_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc10 extends Association src = class2_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, }, MappingStrategyforclass1_name:map_str2MappingStrategyforclass5_name:map_str2MappingStrategyforclass6_name:map_str2MappingStrategyforclass7_name:map_str2AssociationStrategyforassoc1:assoc_str1AssociationStrategyforassoc3:assoc_str1AssociationStrategyforassoc4:assoc_str1AssociationStrategyforassoc7:assoc_str1AssociationStrategyforassoc8:assoc_str1AssociationStrategyforassoc9:assoc_str1AssociationStrategyforassoc10:assoc_str2AssociationStrategyforassoc5:assoc_str2AssociationStrategyforassoc6:assoc_str2, USE OM_name_0 CREATE TABLE `class3_name` ( `c8_at1` c8_at1_type `c3_at6` c3_at6_type `c3_at5` c3_at5_type `c3_at4` c3_at4_type `c3_at3` c3_at3_type `c3_at2` c3_at2_type c3_at1` c3_at1_type NOT NULL c1_at1` c1_at1_type KEY `FK_class3_name_c8_at1_idx` (`c8_at1`) KEY `FK_class3_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c3_at1`), ); CREATE TABLE `class1_name` ( `c1_at1` c1_at2_type(64) `c1_at1` c1_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class2_name` ( `c2_at2` c2_at2_type(64) `c8_at1` c8_at1_type c2_at1` c2_at1_type NOT NULL KEY `FK_class2_name_c8_at1_idx` (`c8_at1`) PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class7_name` ( `c7_at1` c7_at1_type(64) `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc10` ( c3_at1` c3_at1_type NOT NULL c2_at1` c2_at1_type NOT NULL KEY `FK_assoc10_c3_at1_idx` (`c3_at1`) KEY `FK_assoc10_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c3_at1`,`c2_at1`), ); CREATE TABLE `class8_name` ( `c8_at2` c8_at2_type(64) `c2_at2` c2_at2_type(64) ``c8_at1` c8_at1_type NOT NULL PRIMARY KEY (`c8_at1`), ); CREATE TABLE `class5_name` ( `c5_at1` c5_at1_type, `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc5` ( ``c8_at1` c8_at1_type NOT NULL `c2_at1` c2_at1_type NOT NULL KEY `FK_assoc5_c8_at1_idx` (`c8_at1`), KEY `FK_assoc5_c6_at2_idx` (`c6_at2`) PRIMARY KEY (`c8_at1`,`c6_at2`), ); CREATE TABLE `class4_name` ( `c4_at4` c4_at4_type(64) `c4_at2` c4_at2_type(64) `c4_at1` c4_at1_type(64) `c8_at1` c8_at1_type `c6_at2` c6_at2_type `c4_at3` c4_at3_type c1_at1` c1_at1_type KEY `FK_class4_name_c8_at1_idx` (`c8_at1`) KEY `FK_class4_name_c6_at2_idx` (`c6_at2`) KEY `FK_class4_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c4_at3`), ); CREATE TABLE `assoc6` ( `c2_at1` c2_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL `c3_at1` c3_at1_type NOT NULL KEY `FK_assoc6_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c6_at2`,`c1_at1`), ); CREATE TABLE `class6_name` ( `c6_at4` c6_at4_type(64) `c6_at3` c6_at3_type(64) `c6_at1_0` c6_at1_type `c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c6_at2`), ); CREATE TABLE `assoc2` ( `c4_at3` c4_at3_type c2_at1` c2_at1_type NOT NULL KEY `FK_assoc2_c4_at3_idx` (`c4_at3`) KEY `FK_assoc2_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c4_at3`,`c2_at1`), ); ALTER TABLE `class3_name` ADD CONSTRAINT `FK_class3_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_class3_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `class2_name` ADD CONSTRAINT `FK_class2_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ALTER TABLE `assoc10` ADD CONSTRAINT `FK_assoc10_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ADD CONSTRAINT `FK_assoc10_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc5` ADD CONSTRAINT `FK_assoc5_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc5_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `class4_name` ADD CONSTRAINT `FK_class4_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_class4_name_c6_at2` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_class4_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc6` ADD CONSTRAINT `FK_assoc6_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc6_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc2` ADD CONSTRAINT `FK_assoc2_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc2_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE</t>
   </si>
   <si>
@@ -603,6 +600,9 @@
   </si>
   <si>
     <t>module OM_name: 0, open Declaration one sig class1_name extends Class attrSet = c1_at1+c1_at2 id=c1_at1 no parent isAbstract = No } one sig c1_at1 extends c1_at1_type one sig c1_at2 extends c1_at2_type, one sig class2_name extends Class attrSet = c2_at1+c2_at2 id = c2_at1 no parent isAbstract = No } one sig c2_at1 extends c2_at1_type one sig c2_at2 extends c2_at2_type, one sig class3_name extends Class attrSet = c3_at1+c3_at2+c3_at3+c3_at4+c3_at5+c3_at6 id=c3_at1 no parent isAbstract = No } one sig c3_at1 extends c3_at1_type one sig c3_at2 extends c3_at2_type one sig c3_at3 extends c3_at3_type one sig c3_at4 extends c3_at4_type one sig c3_at5 extends c3_at5_type one sig c3_at6 extends c3_at6_type, one sig class4_name extends Class attrSet = c4_at1+c4_at2+c4_at3+c4_at4 id=c4_at3 no parent isAbstract = No } one sig c4_at1 extends c4_at1_type one sig c4_at2 extends c4_at2_type one sig c4_at3 extends c4_at3_type one sig c4_at4 extends c4_at4_type, one sig class5_name extends Class attrSet = c5_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c5_at1 extends c5_at1_type, one sig class6_name extends Class attrSet = c6_at1_0+c6_at2+c6_at3+c6_at4 id=c6_at2 no parent isAbstract = No } one sig c6_at1_0 extends c6_at1_type one sig c6_at2 extends c6_at2_type one sig c6_at3 extends c6_at3_type one sig c6_at4 extends c6_at4_type, one sig class7_name extends Class attrSet = c7_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c7_at1 extends c7_at1_type, one sig class8_name extends Class attrSet = c8_at1+c8_at2+c2_at2+c6_at3 id=c8_at1 no parent isAbstract = No } one sig c8_at1 extends c8_at1_type one sig c8_at1 extends c8_at1_type, one sig assoc1 extends Association src = class8_name dst = class2_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc2 extends Association src = class2_name dst = class4_name, src_multiplicity = src_mlpc2 dst_multiplicity = dst_mlpc, } one sig assoc3 extends Association src = class8_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc4 extends Association src = class8_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc5 extends Association src = class8_name dst = class6_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc6 extends Association src = class6_name dst = class1_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc7 extends Association src = class6_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc8 extends Association src = class1_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc9 extends Association src = class1_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc10 extends Association src = class2_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, }, Mapping Strategy for class1_name : map_str2 Mapping Strategy for class6_name : map_str2 Mapping Strategy for class2_name : map_str1 Mapping Strategy for class5_name : map_str1 Mapping Strategy for class7_name : map_str1 Association Strategy for assoc3 : assoc_str1 Association Strategy for assoc7 : assoc_str1 Association Strategy for assoc8 : assoc_str1 Association Strategy for assoc9 : assoc_str1 Association Strategy for assoc1 : assoc_str2 Association Strategy for assoc10 : assoc_str2 Association Strategy for assoc4 : assoc_str2 Association Strategy for assoc5 : assoc_str2 Association Strategy for assoc6 : assoc_str2 , USE OM_name_0 CREATE TABLE `class3_name` ( `c8_at1` c8_at1_type `c3_at6` c3_at6_type `c3_at5` c3_at5_type `c3_at4` c3_at4_type `c3_at3` c3_at3_type `c3_at2` c3_at2_type c3_at1` c3_at1_type NOT NULL c1_at1` c1_at1_type KEY `FK_class3_name_c8_at1_idx` (`c8_at1`) KEY `FK_class3_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c3_at1`), ); CREATE TABLE `class1_name` ( `c1_at1` c1_at2_type(64) `c1_at1` c1_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class2_name` ( c2_at3` c2_at3_type(64), `c7_at1` c7_at1_type(64) `c5_at1` c5_at1_type, `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc10` ( c3_at1` c3_at1_type NOT NULL c2_at1` c2_at1_type NOT NULL KEY `FK_assoc10_c3_at1_idx` (`c3_at1`) KEY `FK_assoc10_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c3_at1`,`c2_at1`), ); CREATE TABLE `class8_name` ( `c8_at2` c8_at2_type(64) ``c8_at1` c8_at1_type NOT NULL PRIMARY KEY (`c8_at1`), ); CREATE TABLE `assoc5` ( ``c8_at1` c8_at1_type NOT NULL `c2_at1` c2_at1_type NOT NULL KEY `FK_assoc5_c8_at1_idx` (`c8_at1`), KEY `FK_assoc5_c6_at2_idx` (`c6_at2`) PRIMARY KEY (`c8_at1`,`c6_at2`), ); CREATE TABLE `assoc1` ( ``c8_at1` c8_at1_type NOT NULL c2_at1` c2_at1_type NOT NULL KEY `FK_assoc1_c8_at1_idx` (`c8_at1`) KEY `FK_assoc1_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c8_at1`,`c2_at1`) ); CREATE TABLE `assoc4` ( ``c8_at1` c8_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc4_c8_at1_idx` (`c8_at1`) KEY `FK_assoc4_c4_at3_idx` (`c4_at3`) PRIMARY KEY (`c8_at1`,`c4_at3`) ); CREATE TABLE `class4_name` ( `c4_at4` c4_at4_type(64) `c4_at2` c4_at2_type(64) `c4_at1` c4_at1_type(64) `c6_at2` c6_at2_type `c4_at3` c4_at3_type c1_at1` c1_at1_type KEY `FK_class4_name_c6_at2_idx` (`c6_at2`) KEY `FK_class4_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c4_at3`), ); CREATE TABLE `assoc6` ( `c2_at1` c2_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL `c3_at1` c3_at1_type NOT NULL KEY `FK_assoc6_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c6_at2`,`c1_at1`), ); CREATE TABLE `class6_name` ( `c6_at4` c6_at4_type(64) `c6_at3` c6_at3_type(64) `c6_at1_0` c6_at1_type `c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c6_at2`), ); CREATE TABLE `assoc2` ( `c4_at3` c4_at3_type c2_at1` c2_at1_type NOT NULL KEY `FK_assoc2_c4_at3_idx` (`c4_at3`) KEY `FK_assoc2_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c4_at3`,`c2_at1`), ); ALTER TABLE `class3_name` ADD CONSTRAINT `FK_class3_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_class3_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc10` ADD CONSTRAINT `FK_assoc10_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ADD CONSTRAINT `FK_assoc10_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc5` ADD CONSTRAINT `FK_assoc5_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc5_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc1` ADD CONSTRAINT `FK_assoc1_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc1_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE ALTER TABLE `assoc4` ADD CONSTRAINT `FK_assoc4_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc4_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `class4_name` ADD CONSTRAINT `FK_class4_name_c6_at2` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_class4_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc6` ADD CONSTRAINT `FK_assoc6_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc6_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc2` ADD CONSTRAINT `FK_assoc2_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc2_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE,NP</t>
+  </si>
+  <si>
+    <t>module OM_name: 0, open Declaration one sig class1_name extends Class attrSet = c1_at1+c1_at2 id=c1_at1 no parent isAbstract = No } one sig c1_at1 extends c1_at1_type one sig c1_at2 extends c1_at2_type, one sig class2_name extends Class attrSet = c2_at1+c2_at2 id = c2_at1 no parent isAbstract = No } one sig c2_at1 extends c2_at1_type one sig c2_at2 extends c2_at2_type, one sig class3_name extends Class attrSet = c3_at1+c3_at2+c3_at3+c3_at4+c3_at5+c3_at6 id=c3_at1 no parent isAbstract = No } one sig c3_at1 extends c3_at1_type one sig c3_at2 extends c3_at2_type one sig c3_at3 extends c3_at3_type one sig c3_at4 extends c3_at4_type one sig c3_at5 extends c3_at5_type one sig c3_at6 extends c3_at6_type, one sig class4_name extends Class attrSet = c4_at1+c4_at2+c4_at3+c4_at4 id=c4_at3 no parent isAbstract = No } one sig c4_at1 extends c4_at1_type one sig c4_at2 extends c4_at2_type one sig c4_at3 extends c4_at3_type one sig c4_at4 extends c4_at4_type, one sig class5_name extends Class attrSet = c5_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c5_at1 extends c5_at1_type, one sig class6_name extends Class attrSet = c6_at1_0+c6_at2+c6_at3+c6_at4 id=c6_at2 no parent isAbstract = No } one sig c6_at1_0 extends c6_at1_type one sig c6_at2 extends c6_at2_type one sig c6_at3 extends c6_at3_type one sig c6_at4 extends c6_at4_type, one sig class7_name extends Class attrSet = c7_at1 one parent parent in class2_name id=c2_at1 isAbstract = No } one sig c7_at1 extends c7_at1_type, one sig class8_name extends Class attrSet = c8_at1+c8_at2+c2_at2+c6_at3 id=c8_at1 no parent isAbstract = No } one sig c8_at1 extends c8_at1_type one sig c8_at1 extends c8_at1_type, one sig assoc1 extends Association src = class8_name dst = class2_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc2 extends Association src = class2_name dst = class4_name, src_multiplicity = src_mlpc2 dst_multiplicity = dst_mlpc, } one sig assoc3 extends Association src = class8_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc4 extends Association src = class8_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc5 extends Association src = class8_name dst = class6_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc6 extends Association src = class6_name dst = class1_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, } one sig assoc7 extends Association src = class6_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc8 extends Association src = class1_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc9 extends Association src = class1_name dst = class4_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc, } one sig assoc10 extends Association src = class2_name dst = class3_name, src_multiplicity = src_mlpc dst_multiplicity = dst_mlpc2, }, MappingStrategyforclass1_name:map_str2MappingStrategyforclass3_name:map_str2MappingStrategyforclass5_name:map_str2MappingStrategyforclass6_name:map_str2MappingStrategyfoarclass7_name:map_str2AssociationStrategyforassoc1:assoc_str1AssociationStrategyforassoc9:assoc_str1AssociationStrategyforassoc10:assoc_str2AssociationStrategyforassoc3:assoc_str2AssociationStrategyforassoc4:assoc_str2AssociationStrategyforassoc5:assoc_str2AssociationStrategyforassoc6:assoc_str2AssociationStrategyforassoc7:assoc_str2AssociationStrategyforassoc8:assoc_str2​, USE OM_name_0 CREATE TABLE `class3_name` ( `c3_at6` c3_at6_type `c3_at5` c3_at5_type `c3_at4` c3_at4_type `c3_at3` c3_at3_type `c3_at2` c3_at2_type c3_at1` c3_at1_type NOT NULL PRIMARY KEY (`c3_at1`), ); CREATE TABLE `class1_name` ( `c1_at1` c1_at2_type(64) `c1_at1` c1_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class2_name` ( `c2_at2` c2_at2_type(64) `c8_at1` c8_at1_type c2_at1` c2_at1_type NOT NULL KEY `FK_class2_name_c8_at1_idx` (`c8_at1`) PRIMARY KEY (`c1_at1`), ); CREATE TABLE `class7_name` ( `c7_at1` c7_at1_type(64) `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc10` ( c3_at1` c3_at1_type NOT NULL c2_at1` c2_at1_type NOT NULL KEY `FK_assoc10_c3_at1_idx` (`c3_at1`) KEY `FK_assoc10_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c3_at1`,`c2_at1`), ); CREATE TABLE `class8_name` ( `c8_at2` c8_at2_type(64) ``c8_at1` c8_at1_type NOT NULL PRIMARY KEY (`c8_at1`), ); CREATE TABLE `class5_name` ( `c5_at1` c5_at1_type, `c2_at2` c2_at2_type(64) c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c1_at1`), ); CREATE TABLE `assoc7` ( `c2_at1` c2_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc7_c6_at2_idx` (`c6_at2`), KEY `FK_assoc7_c4_at3_idx` (`c4_at3`), PRIMARY KEY (`c6_at2`,`c4_at3`) ); CREATE TABLE `assoc5` ( ``c8_at1` c8_at1_type NOT NULL `c2_at1` c2_at1_type NOT NULL KEY `FK_assoc5_c8_at1_idx` (`c8_at1`), KEY `FK_assoc5_c6_at2_idx` (`c6_at2`) PRIMARY KEY (`c8_at1`,`c6_at2`), ); CREATE TABLE `assoc3` ( ``c8_at1` c8_at1_type NOT NULL c3_at1` c3_at1_type NOT NULL KEY `FK_assoc3_c8_at1_idx` (`c8_at1`) KEY `FK_assoc3_c3_at1_idx` (`c3_at1`) PRIMARY KEY (`c8_at1`,`c3_at1`) ); CREATE TABLE `assoc8` ( c3_at1` c3_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL KEY `FK_assoc8_c3_at1_idx` (`c3_at1`) KEY `FK_assoc8_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c3_at1`,`c1_at1`) ); CREATE TABLE `class4_name` ( `c4_at4` c4_at4_type(64) `c4_at2` c4_at2_type(64) `c4_at1` c4_at1_type(64) `c4_at3` c4_at3_type c1_at1` c1_at1_type KEY `FK_class4_name_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c4_at3`), ); CREATE TABLE `assoc4` ( ``c8_at1` c8_at1_type NOT NULL `c4_at3` c4_at3_type KEY `FK_assoc4_c8_at1_idx` (`c8_at1`) KEY `FK_assoc4_c4_at3_idx` (`c4_at3`) PRIMARY KEY (`c8_at1`,`c4_at3`) ); CREATE TABLE `assoc6` ( `c2_at1` c2_at1_type NOT NULL `c1_at1` c1_at1_type NOT NULL `c3_at1` c3_at1_type NOT NULL KEY `FK_assoc6_c1_at1_idx` (`c1_at1`) PRIMARY KEY (`c6_at2`,`c1_at1`), ); CREATE TABLE `class6_name` ( `c6_at4` c6_at4_type(64) `c6_at3` c6_at3_type(64) `c6_at1_0` c6_at1_type `c2_at1` c2_at1_type NOT NULL PRIMARY KEY (`c6_at2`), ); CREATE TABLE `assoc2` ( `c4_at3` c4_at3_type c2_at1` c2_at1_type NOT NULL KEY `FK_assoc2_c4_at3_idx` (`c4_at3`) KEY `FK_assoc2_c2_at1_idx` (`c2_at1`) PRIMARY KEY (`c4_at3`,`c2_at1`), ); ALTER TABLE `class2_name` ADD CONSTRAINT `FK_class2_name_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ALTER TABLE `assoc10` ADD CONSTRAINT `FK_assoc10_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ADD CONSTRAINT `FK_assoc10_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc7` ADD CONSTRAINT `FK_assoc7_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc7_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc5` ADD CONSTRAINT `FK_assoc5_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc5_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc3` ADD CONSTRAINT `FK_assoc3_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc3_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc8` ADD CONSTRAINT `FK_assoc8_c3_at1` FOREIGN KEY (`c3_at1`) REFERENCES `class3_name` (`c3_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc8_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `class4_name` ADD CONSTRAINT `FK_class4_name_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc4` ADD CONSTRAINT `FK_assoc4_c8_at1` FOREIGN KEY (`c8_at1`) REFERENCES `class8_name` (`c8_at1`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc4_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc6` ADD CONSTRAINT `FK_assoc6_c6_at2` FOREIGN KEY (`c6_at2`) REFERENCES `class6_name` (`c6_at2`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc6_c1_at1` FOREIGN KEY (`c1_at1`) REFERENCES `class1_name` (`c1_at1`) ON DELETE CASCADE ON UPDATE CASCADE, ALTER TABLE `assoc2` ADD CONSTRAINT `FK_assoc2_c4_at3` FOREIGN KEY (`c4_at3`) REFERENCES `class4_name` (`c4_at3`) ON DELETE CASCADE ON UPDATE CASCADE ADD CONSTRAINT `FK_assoc2_c2_at1` FOREIGN KEY (`c2_at1`) REFERENCES `class2_name` (`c2_at1`) ON DELETE CASCADE ON UPDATE CASCADE,P</t>
   </si>
 </sst>
 </file>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE80F2C-09A0-644A-8168-23135C5417CA}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1305,495 +1305,495 @@
         <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>